<commit_message>
changed the exportTimesheet() method to better fit the template that was provided
</commit_message>
<xml_diff>
--- a/writable/templates/badgerspreadsheet.xlsx
+++ b/writable/templates/badgerspreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\PMSBadger\pms-badger\writable\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59804745-A823-47F6-AF39-726CB0B0B2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0012C520-4B4F-421D-9634-97768D934AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{724D3D25-59A1-4492-B610-522F93B5ED80}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{724D3D25-59A1-4492-B610-522F93B5ED80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -699,9 +699,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -712,6 +709,198 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -723,195 +912,6 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1460,7 +1460,7 @@
   <dimension ref="B1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:E16"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,24 +1499,24 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
-      <c r="H3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="H3" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
       <c r="R3" s="5"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
       <c r="R4" s="5"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
@@ -1525,854 +1525,854 @@
     </row>
     <row r="6" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="76"/>
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="76"/>
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
       <c r="R9" s="5"/>
     </row>
     <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="2:18" s="24" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="2:18" s="14" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19" t="s">
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21" t="s">
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="22" t="s">
+      <c r="L11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="21" t="s">
+      <c r="M11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="O11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P11" s="22" t="s">
+      <c r="P11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="Q11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R11" s="23" t="s">
+      <c r="R11" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32">
-        <v>0</v>
-      </c>
-      <c r="L12" s="33">
-        <v>0</v>
-      </c>
-      <c r="M12" s="34">
-        <v>0</v>
-      </c>
-      <c r="N12" s="35">
-        <v>0</v>
-      </c>
-      <c r="O12" s="34">
-        <v>0</v>
-      </c>
-      <c r="P12" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="32">
-        <v>0</v>
-      </c>
-      <c r="R12" s="36">
+      <c r="B12" s="15"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="16">
+        <v>0</v>
+      </c>
+      <c r="L12" s="17">
+        <v>0</v>
+      </c>
+      <c r="M12" s="18">
+        <v>0</v>
+      </c>
+      <c r="N12" s="19">
+        <v>0</v>
+      </c>
+      <c r="O12" s="18">
+        <v>0</v>
+      </c>
+      <c r="P12" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>0</v>
+      </c>
+      <c r="R12" s="20">
         <f t="shared" ref="R12:R29" si="0">SUM(K12:Q12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="32">
-        <v>0</v>
-      </c>
-      <c r="L13" s="33">
-        <v>0</v>
-      </c>
-      <c r="M13" s="34">
-        <v>0</v>
-      </c>
-      <c r="N13" s="35">
-        <v>0</v>
-      </c>
-      <c r="O13" s="34">
-        <v>0</v>
-      </c>
-      <c r="P13" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="32">
-        <v>0</v>
-      </c>
-      <c r="R13" s="36">
+      <c r="B13" s="21"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="16">
+        <v>0</v>
+      </c>
+      <c r="L13" s="17">
+        <v>0</v>
+      </c>
+      <c r="M13" s="18">
+        <v>0</v>
+      </c>
+      <c r="N13" s="19">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
+        <v>0</v>
+      </c>
+      <c r="P13" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>0</v>
+      </c>
+      <c r="R13" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="32">
-        <v>0</v>
-      </c>
-      <c r="L14" s="33">
-        <v>0</v>
-      </c>
-      <c r="M14" s="34">
-        <v>0</v>
-      </c>
-      <c r="N14" s="35">
-        <v>0</v>
-      </c>
-      <c r="O14" s="34">
-        <v>0</v>
-      </c>
-      <c r="P14" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="32">
-        <v>0</v>
-      </c>
-      <c r="R14" s="36">
+      <c r="B14" s="21"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="16">
+        <v>0</v>
+      </c>
+      <c r="L14" s="17">
+        <v>0</v>
+      </c>
+      <c r="M14" s="18">
+        <v>0</v>
+      </c>
+      <c r="N14" s="19">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18">
+        <v>0</v>
+      </c>
+      <c r="P14" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>0</v>
+      </c>
+      <c r="R14" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="32">
-        <v>0</v>
-      </c>
-      <c r="L15" s="33">
-        <v>0</v>
-      </c>
-      <c r="M15" s="34">
-        <v>0</v>
-      </c>
-      <c r="N15" s="35">
-        <v>0</v>
-      </c>
-      <c r="O15" s="34">
-        <v>0</v>
-      </c>
-      <c r="P15" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="32">
-        <v>0</v>
-      </c>
-      <c r="R15" s="36">
+      <c r="B15" s="21"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="16">
+        <v>0</v>
+      </c>
+      <c r="L15" s="17">
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
+        <v>0</v>
+      </c>
+      <c r="N15" s="19">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18">
+        <v>0</v>
+      </c>
+      <c r="P15" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>0</v>
+      </c>
+      <c r="R15" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="32">
-        <v>0</v>
-      </c>
-      <c r="L16" s="33">
-        <v>0</v>
-      </c>
-      <c r="M16" s="34">
-        <v>0</v>
-      </c>
-      <c r="N16" s="35">
-        <v>0</v>
-      </c>
-      <c r="O16" s="34">
-        <v>0</v>
-      </c>
-      <c r="P16" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="32">
-        <v>0</v>
-      </c>
-      <c r="R16" s="36">
+      <c r="B16" s="21"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="17">
+        <v>0</v>
+      </c>
+      <c r="M16" s="18">
+        <v>0</v>
+      </c>
+      <c r="N16" s="19">
+        <v>0</v>
+      </c>
+      <c r="O16" s="18">
+        <v>0</v>
+      </c>
+      <c r="P16" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>0</v>
+      </c>
+      <c r="R16" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="25"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="32">
-        <v>0</v>
-      </c>
-      <c r="L17" s="33">
-        <v>0</v>
-      </c>
-      <c r="M17" s="34">
-        <v>0</v>
-      </c>
-      <c r="N17" s="35">
-        <v>0</v>
-      </c>
-      <c r="O17" s="34">
-        <v>0</v>
-      </c>
-      <c r="P17" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="32">
-        <v>0</v>
-      </c>
-      <c r="R17" s="36">
+      <c r="B17" s="15"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="16">
+        <v>0</v>
+      </c>
+      <c r="L17" s="17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="18">
+        <v>0</v>
+      </c>
+      <c r="N17" s="19">
+        <v>0</v>
+      </c>
+      <c r="O17" s="18">
+        <v>0</v>
+      </c>
+      <c r="P17" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="16">
+        <v>0</v>
+      </c>
+      <c r="R17" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="32">
-        <v>0</v>
-      </c>
-      <c r="L18" s="33">
-        <v>0</v>
-      </c>
-      <c r="M18" s="34">
-        <v>0</v>
-      </c>
-      <c r="N18" s="35">
-        <v>0</v>
-      </c>
-      <c r="O18" s="34">
-        <v>0</v>
-      </c>
-      <c r="P18" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="32">
-        <v>0</v>
-      </c>
-      <c r="R18" s="36">
+      <c r="B18" s="21"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="16">
+        <v>0</v>
+      </c>
+      <c r="L18" s="17">
+        <v>0</v>
+      </c>
+      <c r="M18" s="18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="19">
+        <v>0</v>
+      </c>
+      <c r="O18" s="18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="16">
+        <v>0</v>
+      </c>
+      <c r="R18" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="32">
-        <v>0</v>
-      </c>
-      <c r="L19" s="33">
-        <v>0</v>
-      </c>
-      <c r="M19" s="34">
-        <v>0</v>
-      </c>
-      <c r="N19" s="35">
-        <v>0</v>
-      </c>
-      <c r="O19" s="34">
-        <v>0</v>
-      </c>
-      <c r="P19" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="32">
-        <v>0</v>
-      </c>
-      <c r="R19" s="36">
+      <c r="B19" s="15"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="16">
+        <v>0</v>
+      </c>
+      <c r="L19" s="17">
+        <v>0</v>
+      </c>
+      <c r="M19" s="18">
+        <v>0</v>
+      </c>
+      <c r="N19" s="19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="18">
+        <v>0</v>
+      </c>
+      <c r="P19" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>0</v>
+      </c>
+      <c r="R19" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="32">
-        <v>0</v>
-      </c>
-      <c r="L20" s="33">
-        <v>0</v>
-      </c>
-      <c r="M20" s="34">
-        <v>0</v>
-      </c>
-      <c r="N20" s="35">
-        <v>0</v>
-      </c>
-      <c r="O20" s="34">
-        <v>0</v>
-      </c>
-      <c r="P20" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="32">
-        <v>0</v>
-      </c>
-      <c r="R20" s="36">
+      <c r="B20" s="21"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="16">
+        <v>0</v>
+      </c>
+      <c r="L20" s="17">
+        <v>0</v>
+      </c>
+      <c r="M20" s="18">
+        <v>0</v>
+      </c>
+      <c r="N20" s="19">
+        <v>0</v>
+      </c>
+      <c r="O20" s="18">
+        <v>0</v>
+      </c>
+      <c r="P20" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>0</v>
+      </c>
+      <c r="R20" s="20">
         <f>SUM(K20:Q20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="32">
-        <v>0</v>
-      </c>
-      <c r="L21" s="33">
-        <v>0</v>
-      </c>
-      <c r="M21" s="34">
-        <v>0</v>
-      </c>
-      <c r="N21" s="35">
-        <v>0</v>
-      </c>
-      <c r="O21" s="34">
-        <v>0</v>
-      </c>
-      <c r="P21" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="32">
-        <v>0</v>
-      </c>
-      <c r="R21" s="36">
+      <c r="B21" s="15"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="16">
+        <v>0</v>
+      </c>
+      <c r="L21" s="17">
+        <v>0</v>
+      </c>
+      <c r="M21" s="18">
+        <v>0</v>
+      </c>
+      <c r="N21" s="19">
+        <v>0</v>
+      </c>
+      <c r="O21" s="18">
+        <v>0</v>
+      </c>
+      <c r="P21" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>0</v>
+      </c>
+      <c r="R21" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="37"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="32">
-        <v>0</v>
-      </c>
-      <c r="L22" s="33">
-        <v>0</v>
-      </c>
-      <c r="M22" s="34">
-        <v>0</v>
-      </c>
-      <c r="N22" s="35">
-        <v>0</v>
-      </c>
-      <c r="O22" s="34">
-        <v>0</v>
-      </c>
-      <c r="P22" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="32">
-        <v>0</v>
-      </c>
-      <c r="R22" s="36">
+      <c r="B22" s="21"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="16">
+        <v>0</v>
+      </c>
+      <c r="L22" s="17">
+        <v>0</v>
+      </c>
+      <c r="M22" s="18">
+        <v>0</v>
+      </c>
+      <c r="N22" s="19">
+        <v>0</v>
+      </c>
+      <c r="O22" s="18">
+        <v>0</v>
+      </c>
+      <c r="P22" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>0</v>
+      </c>
+      <c r="R22" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="32">
-        <v>0</v>
-      </c>
-      <c r="L23" s="33">
-        <v>0</v>
-      </c>
-      <c r="M23" s="34">
-        <v>0</v>
-      </c>
-      <c r="N23" s="35">
-        <v>0</v>
-      </c>
-      <c r="O23" s="34">
-        <v>0</v>
-      </c>
-      <c r="P23" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="32">
-        <v>0</v>
-      </c>
-      <c r="R23" s="36">
+      <c r="B23" s="15"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="16">
+        <v>0</v>
+      </c>
+      <c r="L23" s="17">
+        <v>0</v>
+      </c>
+      <c r="M23" s="18">
+        <v>0</v>
+      </c>
+      <c r="N23" s="19">
+        <v>0</v>
+      </c>
+      <c r="O23" s="18">
+        <v>0</v>
+      </c>
+      <c r="P23" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="16">
+        <v>0</v>
+      </c>
+      <c r="R23" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="37"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="32">
-        <v>0</v>
-      </c>
-      <c r="L24" s="33">
-        <v>0</v>
-      </c>
-      <c r="M24" s="34">
-        <v>0</v>
-      </c>
-      <c r="N24" s="35">
-        <v>0</v>
-      </c>
-      <c r="O24" s="34">
-        <v>0</v>
-      </c>
-      <c r="P24" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="32">
-        <v>0</v>
-      </c>
-      <c r="R24" s="36">
+      <c r="B24" s="21"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="16">
+        <v>0</v>
+      </c>
+      <c r="L24" s="17">
+        <v>0</v>
+      </c>
+      <c r="M24" s="18">
+        <v>0</v>
+      </c>
+      <c r="N24" s="19">
+        <v>0</v>
+      </c>
+      <c r="O24" s="18">
+        <v>0</v>
+      </c>
+      <c r="P24" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="16">
+        <v>0</v>
+      </c>
+      <c r="R24" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="32">
-        <v>0</v>
-      </c>
-      <c r="L25" s="33">
-        <v>0</v>
-      </c>
-      <c r="M25" s="34">
-        <v>0</v>
-      </c>
-      <c r="N25" s="35">
-        <v>0</v>
-      </c>
-      <c r="O25" s="34">
-        <v>0</v>
-      </c>
-      <c r="P25" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="32">
-        <v>0</v>
-      </c>
-      <c r="R25" s="36">
+      <c r="B25" s="21"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="16">
+        <v>0</v>
+      </c>
+      <c r="L25" s="17">
+        <v>0</v>
+      </c>
+      <c r="M25" s="18">
+        <v>0</v>
+      </c>
+      <c r="N25" s="19">
+        <v>0</v>
+      </c>
+      <c r="O25" s="18">
+        <v>0</v>
+      </c>
+      <c r="P25" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="16">
+        <v>0</v>
+      </c>
+      <c r="R25" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="37"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="32">
-        <v>0</v>
-      </c>
-      <c r="L26" s="33">
-        <v>0</v>
-      </c>
-      <c r="M26" s="34">
-        <v>0</v>
-      </c>
-      <c r="N26" s="35">
-        <v>0</v>
-      </c>
-      <c r="O26" s="34">
-        <v>0</v>
-      </c>
-      <c r="P26" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="32">
-        <v>0</v>
-      </c>
-      <c r="R26" s="36">
+      <c r="B26" s="21"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="16">
+        <v>0</v>
+      </c>
+      <c r="L26" s="17">
+        <v>0</v>
+      </c>
+      <c r="M26" s="18">
+        <v>0</v>
+      </c>
+      <c r="N26" s="19">
+        <v>0</v>
+      </c>
+      <c r="O26" s="18">
+        <v>0</v>
+      </c>
+      <c r="P26" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>0</v>
+      </c>
+      <c r="R26" s="20">
         <f>SUM(K26:Q26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="37"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="32"/>
-      <c r="R27" s="36">
+      <c r="B27" s="21"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="37"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="32"/>
-      <c r="R28" s="36">
+      <c r="B28" s="21"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="56" t="s">
+      <c r="D29" s="34"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="59">
-        <v>0</v>
-      </c>
-      <c r="L29" s="60">
-        <v>0</v>
-      </c>
-      <c r="M29" s="61">
-        <v>0</v>
-      </c>
-      <c r="N29" s="62">
-        <v>0</v>
-      </c>
-      <c r="O29" s="61">
-        <v>0</v>
-      </c>
-      <c r="P29" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="59">
-        <v>0</v>
-      </c>
-      <c r="R29" s="63">
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="23">
+        <v>0</v>
+      </c>
+      <c r="L29" s="24">
+        <v>0</v>
+      </c>
+      <c r="M29" s="25">
+        <v>0</v>
+      </c>
+      <c r="N29" s="26">
+        <v>0</v>
+      </c>
+      <c r="O29" s="25">
+        <v>0</v>
+      </c>
+      <c r="P29" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="23">
+        <v>0</v>
+      </c>
+      <c r="R29" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="67">
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="28">
         <f t="shared" ref="K30:Q30" si="1">SUM(K12:K29)</f>
         <v>0</v>
       </c>
-      <c r="L30" s="68">
+      <c r="L30" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M30" s="69">
+      <c r="M30" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N30" s="70">
+      <c r="N30" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O30" s="69">
+      <c r="O30" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P30" s="70">
+      <c r="P30" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="67">
+      <c r="Q30" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R30" s="71"/>
+      <c r="R30" s="32"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="73"/>
-      <c r="N31" s="73"/>
-      <c r="O31" s="73"/>
-      <c r="P31" s="73"/>
-      <c r="Q31" s="74"/>
-      <c r="R31" s="74">
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="44">
         <f>K30+L30+M30+N30+O30+P30+Q30</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="75"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="76"/>
-      <c r="K32" s="76"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="76"/>
-      <c r="P32" s="76"/>
-      <c r="Q32" s="77"/>
-      <c r="R32" s="77"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="47"/>
+      <c r="R32" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="B31:Q32"/>
-    <mergeCell ref="R31:R32"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="H3:M4"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:J25"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="F26:J26"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="F27:J27"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="F28:J28"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="H3:M4"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="B31:Q32"/>
+    <mergeCell ref="R31:R32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
badgerspreadsheet.xlsx had a slight bug fixed it
</commit_message>
<xml_diff>
--- a/writable/templates/badgerspreadsheet.xlsx
+++ b/writable/templates/badgerspreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\PMSBadger\pms-badger\writable\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0012C520-4B4F-421D-9634-97768D934AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B8B020-B4CD-4095-B8BC-CAFD0E1A8BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{724D3D25-59A1-4492-B610-522F93B5ED80}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{724D3D25-59A1-4492-B610-522F93B5ED80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -778,6 +778,96 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,96 +912,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1460,7 +1460,7 @@
   <dimension ref="B1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,24 +1499,24 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
-      <c r="H3" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
+      <c r="H3" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
       <c r="R3" s="5"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
       <c r="R4" s="5"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
@@ -1525,24 +1525,24 @@
     </row>
     <row r="6" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="I6" s="74" t="s">
+      <c r="I6" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="74"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="76"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37"/>
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="74" t="s">
+      <c r="I7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="74"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="76"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="37"/>
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -1559,14 +1559,14 @@
       <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="74" t="s">
+      <c r="I9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="77"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
       <c r="R9" s="5"/>
     </row>
     <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1577,18 +1577,18 @@
       <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="65" t="s">
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="66"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="42"/>
       <c r="K11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1616,14 +1616,14 @@
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="72"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="16">
         <v>0</v>
       </c>
@@ -1652,14 +1652,14 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
       <c r="K13" s="16">
         <v>0</v>
       </c>
@@ -1688,14 +1688,14 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="54"/>
       <c r="K14" s="16">
         <v>0</v>
       </c>
@@ -1724,14 +1724,14 @@
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="53"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="54"/>
       <c r="K15" s="16">
         <v>0</v>
       </c>
@@ -1760,14 +1760,14 @@
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="16">
         <v>0</v>
       </c>
@@ -1795,14 +1795,14 @@
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="62"/>
       <c r="K17" s="16">
         <v>0</v>
       </c>
@@ -1831,14 +1831,14 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="59"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="62"/>
       <c r="K18" s="16">
         <v>0</v>
       </c>
@@ -1867,14 +1867,14 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="62"/>
       <c r="K19" s="16">
         <v>0</v>
       </c>
@@ -1903,14 +1903,14 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="59"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="62"/>
       <c r="K20" s="16">
         <v>0</v>
       </c>
@@ -1939,14 +1939,14 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="62"/>
       <c r="K21" s="16">
         <v>0</v>
       </c>
@@ -1975,14 +1975,14 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="21"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="59"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="62"/>
       <c r="K22" s="16">
         <v>0</v>
       </c>
@@ -2011,14 +2011,14 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="62"/>
       <c r="K23" s="16">
         <v>0</v>
       </c>
@@ -2047,14 +2047,14 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="53"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="54"/>
       <c r="K24" s="16">
         <v>0</v>
       </c>
@@ -2077,19 +2077,19 @@
         <v>0</v>
       </c>
       <c r="R24" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="53"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="54"/>
       <c r="K25" s="16">
         <v>0</v>
       </c>
@@ -2118,14 +2118,14 @@
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="53"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="16">
         <v>0</v>
       </c>
@@ -2154,14 +2154,14 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="53"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="54"/>
       <c r="K27" s="16"/>
       <c r="L27" s="17"/>
       <c r="M27" s="18"/>
@@ -2176,14 +2176,14 @@
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="21"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="53"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="54"/>
       <c r="K28" s="16"/>
       <c r="L28" s="17"/>
       <c r="M28" s="18"/>
@@ -2200,18 +2200,18 @@
       <c r="B29" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36" t="s">
+      <c r="D29" s="64"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="38"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="68"/>
       <c r="K29" s="23">
         <v>0</v>
       </c>
@@ -2239,17 +2239,17 @@
       </c>
     </row>
     <row r="30" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="41"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="71"/>
       <c r="K30" s="28">
         <f t="shared" ref="K30:Q30" si="1">SUM(K12:K29)</f>
         <v>0</v>
@@ -2281,50 +2281,91 @@
       <c r="R30" s="32"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44">
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="73"/>
+      <c r="M31" s="73"/>
+      <c r="N31" s="73"/>
+      <c r="O31" s="73"/>
+      <c r="P31" s="73"/>
+      <c r="Q31" s="74"/>
+      <c r="R31" s="74">
         <f>K30+L30+M30+N30+O30+P30+Q30</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="47"/>
-      <c r="R32" s="47"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="76"/>
+      <c r="L32" s="76"/>
+      <c r="M32" s="76"/>
+      <c r="N32" s="76"/>
+      <c r="O32" s="76"/>
+      <c r="P32" s="76"/>
+      <c r="Q32" s="77"/>
+      <c r="R32" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="B31:Q32"/>
+    <mergeCell ref="R31:R32"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:J26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:J13"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="H3:M4"/>
@@ -2332,47 +2373,6 @@
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:J26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="B31:Q32"/>
-    <mergeCell ref="R31:R32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>